<commit_message>
update parts list with sensors and links
</commit_message>
<xml_diff>
--- a/System Integration/electrical_parts_list.xlsx
+++ b/System Integration/electrical_parts_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevSpace\Projects\FormulaAV2020\Hardware_Algo\System Integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290CBE63-9B15-4BCA-8F49-38AD59B31469}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094381FA-5134-4745-892C-7EE3CA342745}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15540" xr2:uid="{FD6B09E7-CAE9-46B4-9648-433F28AAFF9C}"/>
+    <workbookView xWindow="-19310" yWindow="2930" windowWidth="19420" windowHeight="10560" xr2:uid="{FD6B09E7-CAE9-46B4-9648-433F28AAFF9C}"/>
   </bookViews>
   <sheets>
     <sheet name="power" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="167">
   <si>
     <t>protaction circuit</t>
   </si>
@@ -296,9 +296,6 @@
     <t>EBS Air Pressure</t>
   </si>
   <si>
-    <t>Coolnet temperature</t>
-  </si>
-  <si>
     <t>DRS pos.</t>
   </si>
   <si>
@@ -531,6 +528,15 @@
   </si>
   <si>
     <t>7-60V, 3 tiny temperture sensors are provided too</t>
+  </si>
+  <si>
+    <t>Coolnet temperature &amp; Pressure</t>
+  </si>
+  <si>
+    <t>https://www.kasensors.com/sites/default/files/downloads/ASHT%20High%20Performance%20Low%20Range%20Pressure%20%26%20Temperature%2006.20.pdf</t>
+  </si>
+  <si>
+    <t>KA sensors ASHT-A5000-5A1-ABF-050-000</t>
   </si>
 </sst>
 </file>
@@ -689,9 +695,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -700,9 +703,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -735,6 +735,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -1051,125 +1057,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99AB1913-3ACA-4A36-ADF0-5064DFF99C18}">
-  <dimension ref="A1:Y71"/>
+  <dimension ref="A1:Y70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="8" customWidth="1"/>
-    <col min="2" max="2" width="20" style="21" customWidth="1"/>
-    <col min="3" max="3" width="33.54296875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.54296875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="38.7265625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="10.90625" customWidth="1"/>
-    <col min="8" max="8" width="4.90625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="18.81640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="17.6328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20" style="19" customWidth="1"/>
+    <col min="3" max="3" width="37.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="4" customWidth="1"/>
     <col min="11" max="11" width="17" style="4" customWidth="1"/>
-    <col min="12" max="12" width="18.7265625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" style="4" customWidth="1"/>
     <col min="13" max="13" width="18" style="4" customWidth="1"/>
-    <col min="14" max="14" width="16.453125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="17.453125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="16.54296875" style="4" customWidth="1"/>
-    <col min="17" max="16384" width="9.1796875" style="4"/>
+    <col min="14" max="14" width="16.42578125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="19" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8"/>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="9" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="9" t="s">
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9" t="s">
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9" t="s">
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-    </row>
-    <row r="2" spans="1:25" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+    </row>
+    <row r="2" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>66</v>
       </c>
       <c r="G2" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="I2" s="14" t="s">
+      <c r="H2" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="N2" s="14" t="s">
+      <c r="M2" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="P2" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="P2" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>123</v>
+    </row>
+    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>122</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>36</v>
@@ -1183,7 +1189,7 @@
       <c r="F3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="24" t="str">
+      <c r="G3" s="22" t="str">
         <f>HYPERLINK(H3,"Datasheet")</f>
         <v>Datasheet</v>
       </c>
@@ -1201,13 +1207,13 @@
       </c>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:25" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
-      <c r="B4" s="21" t="s">
+    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>160</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>161</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -1216,9 +1222,9 @@
         <v>1</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="G4" s="24"/>
+        <v>161</v>
+      </c>
+      <c r="G4" s="22"/>
       <c r="I4" s="4">
         <v>12</v>
       </c>
@@ -1227,13 +1233,13 @@
       </c>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
-      <c r="B5" s="21" t="s">
-        <v>122</v>
+    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1242,10 +1248,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="G5" s="24" t="str">
-        <f t="shared" ref="G5:G68" si="0">HYPERLINK(H5,"Datasheet")</f>
+        <v>158</v>
+      </c>
+      <c r="G5" s="22" t="str">
+        <f t="shared" ref="G5:G67" si="0">HYPERLINK(H5,"Datasheet")</f>
         <v>Datasheet</v>
       </c>
       <c r="I5" s="4">
@@ -1256,10 +1262,10 @@
       </c>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:25" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
-      <c r="B6" s="21" t="s">
-        <v>124</v>
+    <row r="6" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="19" t="s">
+        <v>123</v>
       </c>
       <c r="D6" s="4">
         <v>3</v>
@@ -1270,29 +1276,29 @@
       <c r="F6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="24" t="str">
+      <c r="G6" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
-      <c r="B7" s="21" t="s">
-        <v>125</v>
+    <row r="7" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
+      <c r="B7" s="19" t="s">
+        <v>124</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>110</v>
+      <c r="G7" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="I7" s="4">
         <v>24</v>
@@ -1302,23 +1308,23 @@
       </c>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
-      <c r="B8" s="21" t="s">
-        <v>126</v>
+    <row r="8" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="19" t="s">
+        <v>125</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>110</v>
+      <c r="G8" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="I8" s="4">
         <v>24</v>
@@ -1328,23 +1334,23 @@
       </c>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:25" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="9"/>
-      <c r="B9" s="21" t="s">
-        <v>127</v>
+    <row r="9" spans="1:25" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="23"/>
+      <c r="B9" s="19" t="s">
+        <v>126</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>110</v>
+      <c r="G9" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>109</v>
       </c>
       <c r="I9" s="4">
         <v>24</v>
@@ -1354,23 +1360,23 @@
       </c>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="9"/>
-      <c r="B10" s="21" t="s">
+    <row r="10" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="23"/>
+      <c r="B10" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>115</v>
       </c>
       <c r="I10" s="4">
         <v>12</v>
@@ -1383,10 +1389,10 @@
       </c>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
-      <c r="B11" s="21" t="s">
-        <v>128</v>
+    <row r="11" spans="1:25" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23"/>
+      <c r="B11" s="19" t="s">
+        <v>127</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>43</v>
@@ -1394,7 +1400,7 @@
       <c r="F11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="24" t="str">
+      <c r="G11" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
@@ -1406,9 +1412,9 @@
       </c>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="9"/>
-      <c r="B12" s="21" t="s">
+    <row r="12" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1417,7 +1423,7 @@
       <c r="F12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="24" t="str">
+      <c r="G12" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
@@ -1430,46 +1436,46 @@
       <c r="L12" s="5"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
-      <c r="B13" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="G13" s="24" t="str">
+    <row r="13" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="9"/>
-      <c r="B14" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="G14" s="24" t="str">
+    <row r="14" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
+      <c r="B14" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="9"/>
-      <c r="B15" s="21" t="s">
+    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>111</v>
+      <c r="C15" s="10" t="s">
+        <v>110</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>112</v>
+      <c r="G15" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>111</v>
       </c>
       <c r="I15" s="4">
         <v>24</v>
@@ -1480,9 +1486,9 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
-      <c r="B16" s="21" t="s">
+    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="19" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1491,12 +1497,12 @@
       <c r="F16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>163</v>
+      <c r="G16" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>162</v>
       </c>
       <c r="I16" s="4">
         <v>24</v>
@@ -1508,24 +1514,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="9"/>
-      <c r="B17" s="21" t="s">
-        <v>132</v>
+    <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
+      <c r="B17" s="19" t="s">
+        <v>131</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="G17" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H17" s="11" t="s">
+      <c r="E17" s="10"/>
+      <c r="F17" s="10" t="s">
         <v>163</v>
+      </c>
+      <c r="G17" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>162</v>
       </c>
       <c r="I17" s="4">
         <v>24</v>
@@ -1534,86 +1540,86 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
-      <c r="B18" s="21" t="s">
+    <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
+      <c r="B18" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H18" s="10" t="s">
         <v>134</v>
-      </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>135</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K18" s="11"/>
-    </row>
-    <row r="19" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="9"/>
-      <c r="B19" s="21" t="s">
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="23"/>
+      <c r="B19" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="G19" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>143</v>
+      <c r="G19" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>142</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
-      <c r="B20" s="21" t="s">
+    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="23"/>
+      <c r="B20" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="G20" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>142</v>
+      <c r="G20" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>141</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
-      <c r="G21" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" s="15" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="9"/>
-      <c r="B22" s="22"/>
-      <c r="G22" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="9" t="s">
+    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
+      <c r="G21" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="23"/>
+      <c r="B22" s="20"/>
+      <c r="G22" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="19" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="4">
@@ -1622,7 +1628,7 @@
       <c r="F23" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G23" s="24" t="str">
+      <c r="G23" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
@@ -1632,11 +1638,11 @@
       <c r="K23" s="7">
         <v>200</v>
       </c>
-      <c r="L23" s="15"/>
-    </row>
-    <row r="24" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="9"/>
-      <c r="B24" s="21" t="s">
+      <c r="L23" s="13"/>
+    </row>
+    <row r="24" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="23"/>
+      <c r="B24" s="19" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="4">
@@ -1645,7 +1651,7 @@
       <c r="F24" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="24" t="str">
+      <c r="G24" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
@@ -1655,24 +1661,24 @@
       <c r="K24" s="7">
         <v>100</v>
       </c>
-      <c r="L24" s="15"/>
-    </row>
-    <row r="25" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="9"/>
-      <c r="B25" s="21" t="s">
-        <v>116</v>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="25" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="23"/>
+      <c r="B25" s="19" t="s">
+        <v>115</v>
       </c>
       <c r="D25" s="4">
         <v>1</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H25" s="10"/>
+      <c r="G25" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H25" s="9"/>
       <c r="I25" s="4">
         <v>24</v>
       </c>
@@ -1680,121 +1686,121 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
-      <c r="B26" s="21" t="s">
-        <v>119</v>
+    <row r="26" spans="1:13" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
+      <c r="B26" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="D26" s="4">
         <v>4</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G26" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H26" s="10"/>
+      <c r="G26" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H26" s="9"/>
       <c r="I26" s="4">
         <v>12</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="K26" s="11">
+      <c r="K26" s="10">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="9"/>
-      <c r="B27" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>145</v>
+    <row r="27" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="23"/>
+      <c r="B27" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>144</v>
       </c>
       <c r="D27" s="4">
         <v>2</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>146</v>
+      <c r="F27" s="10"/>
+      <c r="G27" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>145</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="K27" s="11"/>
-    </row>
-    <row r="28" spans="1:13" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="9"/>
-      <c r="B28" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="F28" s="16" t="s">
+      <c r="K27" s="10"/>
+    </row>
+    <row r="28" spans="1:13" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="23"/>
+      <c r="B28" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="F28" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H28" s="16"/>
+      <c r="G28" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H28" s="14"/>
       <c r="I28" s="4">
         <v>24</v>
       </c>
-      <c r="K28" s="17">
+      <c r="K28" s="15">
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
-      <c r="B29" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15" t="s">
+    <row r="29" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
+      <c r="B29" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G29" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15">
+      <c r="G29" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13">
         <v>12</v>
       </c>
-      <c r="J29" s="15">
+      <c r="J29" s="13">
         <v>3.4</v>
       </c>
-      <c r="K29" s="15">
+      <c r="K29" s="13">
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="9"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H30" s="10"/>
-      <c r="K30" s="11"/>
-    </row>
-    <row r="31" spans="1:13" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="9"/>
-      <c r="B31" s="21" t="s">
+    <row r="30" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="K30" s="10"/>
+    </row>
+    <row r="31" spans="1:13" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="19" t="s">
         <v>45</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G31" s="24" t="str">
+      <c r="G31" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
@@ -1805,15 +1811,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
+    <row r="32" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>152</v>
+      <c r="C32" s="11" t="s">
+        <v>151</v>
       </c>
       <c r="D32" s="4">
         <v>2</v>
@@ -1822,24 +1828,24 @@
         <v>3</v>
       </c>
       <c r="F32"/>
-      <c r="G32" s="24" t="str">
+      <c r="G32" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="9"/>
-      <c r="B33" s="21" t="s">
+    <row r="33" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="23"/>
+      <c r="B33" s="19" t="s">
         <v>79</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D33" s="4">
         <v>4</v>
@@ -1848,24 +1854,24 @@
         <v>5</v>
       </c>
       <c r="F33"/>
-      <c r="G33" s="24" t="str">
+      <c r="G33" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="9"/>
-      <c r="B34" s="21" t="s">
+    <row r="34" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
+      <c r="B34" s="19" t="s">
         <v>81</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
@@ -1873,15 +1879,15 @@
       <c r="E34" s="4">
         <v>1</v>
       </c>
-      <c r="F34" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="G34" s="24" t="str">
+      <c r="F34" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="G34" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I34" s="4">
         <v>24</v>
@@ -1890,16 +1896,16 @@
         <v>0.6</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="9"/>
-      <c r="B35" s="21" t="s">
-        <v>93</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="23"/>
+      <c r="B35" s="19" t="s">
+        <v>92</v>
       </c>
       <c r="C35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D35" s="4">
         <v>2</v>
@@ -1907,25 +1913,25 @@
       <c r="E35" s="4">
         <v>2</v>
       </c>
-      <c r="F35" s="18"/>
-      <c r="G35" s="24" t="str">
+      <c r="F35" s="16"/>
+      <c r="G35" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M35" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="9"/>
-      <c r="B36" s="21" t="s">
+    <row r="36" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
+      <c r="B36" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D36" s="4">
         <v>4</v>
@@ -1933,68 +1939,71 @@
       <c r="E36" s="4">
         <v>3</v>
       </c>
-      <c r="F36" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="G36" s="24" t="str">
+      <c r="F36" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="G36" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M36" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="9"/>
-      <c r="B37" s="21" t="s">
+    <row r="37" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
+      <c r="B37" s="19" t="s">
         <v>83</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D37" s="4">
         <v>1</v>
       </c>
-      <c r="G37" s="24" t="str">
+      <c r="G37" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="9"/>
-      <c r="B38" s="21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
+      <c r="B38" s="19" t="s">
         <v>84</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D38" s="4">
         <v>1</v>
       </c>
-      <c r="G38" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
+      <c r="G38" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="M38" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="9"/>
-      <c r="B39" s="21" t="s">
+    <row r="39" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="23"/>
+      <c r="B39" s="19" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D39" s="4">
         <v>4</v>
@@ -2002,350 +2011,346 @@
       <c r="E39" s="4">
         <v>0</v>
       </c>
-      <c r="G39" s="24" t="str">
+      <c r="G39" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M39" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="9"/>
+    <row r="40" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
+      <c r="B40" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>166</v>
+      </c>
       <c r="D40" s="4">
+        <v>2</v>
+      </c>
+      <c r="G40" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="23"/>
+      <c r="B41" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D41" s="4">
         <v>1</v>
       </c>
-      <c r="G40" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="9"/>
-      <c r="B41" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="D41" s="4">
-        <v>2</v>
-      </c>
-      <c r="G41" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="9"/>
-      <c r="B42" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>76</v>
+      <c r="G41" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="23"/>
+      <c r="B42" s="19" t="s">
+        <v>89</v>
       </c>
       <c r="D42" s="4">
         <v>1</v>
       </c>
-      <c r="G42" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="9"/>
-      <c r="B43" s="21" t="s">
+      <c r="G42" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="M42" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="4">
-        <v>1</v>
-      </c>
-      <c r="G43" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="M43" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="9"/>
-      <c r="G44" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="9" t="s">
+    </row>
+    <row r="43" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="23"/>
+      <c r="G43" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="23" t="s">
+      <c r="B44" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="D44" s="4">
+        <v>3</v>
+      </c>
+      <c r="G44" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H44" s="10" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="23"/>
+      <c r="B45" s="19" t="s">
+        <v>143</v>
       </c>
       <c r="D45" s="4">
         <v>3</v>
       </c>
-      <c r="G45" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H45" s="11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="9"/>
-      <c r="B46" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="D46" s="4">
+      <c r="G45" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G46" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="23"/>
+      <c r="G47" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
+      <c r="G48" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
+      <c r="G49" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
+      <c r="G50" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
+      <c r="G51" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G52" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L52" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="23"/>
+      <c r="B53" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="9"/>
-      <c r="B47" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G47" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="9"/>
-      <c r="G48" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="9"/>
-      <c r="G49" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="9"/>
-      <c r="G50" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="9"/>
-      <c r="G51" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="9"/>
-      <c r="G52" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" s="14" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B53" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C53" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G53" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="I53" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J53" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="L53" s="14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="9"/>
-      <c r="B54" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G54" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="I54" s="4" t="s">
+      <c r="G53" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="I53" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L54" s="4" t="s">
+      <c r="L53" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="9"/>
-      <c r="B55" s="21" t="s">
+    <row r="54" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="23"/>
+      <c r="B54" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G55" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="9"/>
-      <c r="G56" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="9" t="s">
+      <c r="G54" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
+      <c r="G55" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="B56" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="B57" s="21" t="s">
+      <c r="G56" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="23"/>
+      <c r="B57" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="G57" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="9"/>
-      <c r="B58" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="G58" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="9" t="s">
+      <c r="G57" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="G59" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="9"/>
-      <c r="G60" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="9"/>
-      <c r="G61" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="9"/>
-      <c r="G62" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="9"/>
-      <c r="G63" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="9"/>
-      <c r="G64" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="9"/>
-      <c r="G65" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="9"/>
-      <c r="G66" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="9"/>
-      <c r="G67" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="9"/>
-      <c r="G68" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B69" s="22" t="s">
+      <c r="G58" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="23"/>
+      <c r="G59" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="23"/>
+      <c r="G60" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="23"/>
+      <c r="G61" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="23"/>
+      <c r="G62" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="23"/>
+      <c r="G63" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="23"/>
+      <c r="G64" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="23"/>
+      <c r="G65" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="23"/>
+      <c r="G66" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="23"/>
+      <c r="G67" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C69" s="15"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="15"/>
-      <c r="F69" s="15"/>
-      <c r="H69" s="15"/>
-      <c r="I69" s="15"/>
-      <c r="J69" s="15"/>
-      <c r="K69" s="15">
-        <f>SUM(K3:K68)</f>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="13">
+        <f>SUM(K3:K67)</f>
         <v>1282.6599999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B70" s="22" t="s">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B69" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-      <c r="E70" s="15"/>
-      <c r="F70" s="15"/>
-      <c r="H70" s="15"/>
-      <c r="I70" s="15"/>
-      <c r="J70" s="15"/>
-      <c r="K70" s="15">
-        <f>SUMIF(I3:I68,12,K3:K68)</f>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="13">
+        <f>SUMIF(I3:I67,12,K3:K67)</f>
         <v>668.8</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B71" s="21" t="s">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B70" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="K71" s="15">
-        <f>SUMIF(I3:I68,24,K3:K68)</f>
+      <c r="K70" s="13">
+        <f>SUMIF(I3:I67,24,K3:K67)</f>
         <v>613.86</v>
       </c>
     </row>
@@ -2356,13 +2361,13 @@
     <mergeCell ref="M1:P1"/>
     <mergeCell ref="Q1:U1"/>
     <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="A59:A68"/>
+    <mergeCell ref="A58:A67"/>
     <mergeCell ref="A3:A22"/>
     <mergeCell ref="A23:A31"/>
-    <mergeCell ref="A32:A44"/>
-    <mergeCell ref="A45:A52"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A32:A43"/>
+    <mergeCell ref="A44:A51"/>
+    <mergeCell ref="A52:A55"/>
+    <mergeCell ref="A56:A57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2377,83 +2382,83 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" customWidth="1"/>
-    <col min="2" max="2" width="32.81640625" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2461,37 +2466,37 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -2509,117 +2514,117 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -2637,15 +2642,15 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" customWidth="1"/>
-    <col min="2" max="2" width="27.1796875" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" customWidth="1"/>
-    <col min="4" max="4" width="26.26953125" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
@@ -2659,7 +2664,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2673,7 +2678,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2681,7 +2686,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2689,7 +2694,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2697,12 +2702,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2710,77 +2715,77 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
mid work commit for saving
</commit_message>
<xml_diff>
--- a/System Integration/electrical_parts_list.xlsx
+++ b/System Integration/electrical_parts_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DevSpace\Projects\FormulaAV2020\Hardware_Algo\System Integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094381FA-5134-4745-892C-7EE3CA342745}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709A625E-CEAE-4157-9442-926CA454C281}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="2930" windowWidth="19420" windowHeight="10560" xr2:uid="{FD6B09E7-CAE9-46B4-9648-433F28AAFF9C}"/>
+    <workbookView xWindow="1190" yWindow="1180" windowWidth="14400" windowHeight="7460" xr2:uid="{FD6B09E7-CAE9-46B4-9648-433F28AAFF9C}"/>
   </bookViews>
   <sheets>
     <sheet name="power" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="172">
   <si>
     <t>protaction circuit</t>
   </si>
@@ -161,9 +161,6 @@
     <t>current peak 130A/200us</t>
   </si>
   <si>
-    <t>SPAL VA32-A101-62A 12V 3.4A-MAX</t>
-  </si>
-  <si>
     <t>power by the autonomuos pc. Wattage include in pc power</t>
   </si>
   <si>
@@ -537,6 +534,24 @@
   </si>
   <si>
     <t>KA sensors ASHT-A5000-5A1-ABF-050-000</t>
+  </si>
+  <si>
+    <t>http://www.xq-power.com/XQ-S42/show_54.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12V 3.4A-MAX</t>
+  </si>
+  <si>
+    <t>SPAL VA32-A101-62A</t>
+  </si>
+  <si>
+    <t>https://www.spalautomotive.it/axial-fans/VA32-A100-62S/33179</t>
+  </si>
+  <si>
+    <t>http://www.aquatec.com/documents/downloads/550%20Series%2024VDC%205.15%20GPM.pdf</t>
+  </si>
+  <si>
+    <t>Aquatec 5511-1012-b736</t>
   </si>
 </sst>
 </file>
@@ -671,7 +686,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -735,6 +750,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1060,90 +1078,90 @@
   <dimension ref="A1:Y70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" style="8" customWidth="1"/>
     <col min="2" max="2" width="20" style="19" customWidth="1"/>
-    <col min="3" max="3" width="37.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="38.7109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38.7265625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" customWidth="1"/>
+    <col min="8" max="8" width="4.81640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="17.54296875" style="4" customWidth="1"/>
     <col min="11" max="11" width="17" style="4" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="18.7265625" style="4" customWidth="1"/>
     <col min="13" max="13" width="18" style="4" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" style="4" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="4" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="4"/>
+    <col min="14" max="14" width="16.453125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.453125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="16.54296875" style="4" customWidth="1"/>
+    <col min="17" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="23" t="s">
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="23" t="s">
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-    </row>
-    <row r="2" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+    </row>
+    <row r="2" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>37</v>
@@ -1158,24 +1176,24 @@
         <v>0</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="P2" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>119</v>
+    </row>
+    <row r="3" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="24" t="s">
+        <v>118</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>36</v>
@@ -1207,13 +1225,13 @@
       </c>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+    <row r="4" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="24"/>
       <c r="B4" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -1222,7 +1240,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G4" s="22"/>
       <c r="I4" s="4">
@@ -1233,13 +1251,13 @@
       </c>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+    <row r="5" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="24"/>
       <c r="B5" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1248,7 +1266,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G5" s="22" t="str">
         <f t="shared" ref="G5:G67" si="0">HYPERLINK(H5,"Datasheet")</f>
@@ -1262,10 +1280,10 @@
       </c>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:25" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+    <row r="6" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="24"/>
       <c r="B6" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D6" s="4">
         <v>3</v>
@@ -1274,7 +1292,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6" s="22" t="str">
         <f t="shared" si="0"/>
@@ -1282,23 +1300,23 @@
       </c>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:25" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
+    <row r="7" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="24"/>
       <c r="B7" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H7" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="I7" s="4">
         <v>24</v>
@@ -1308,23 +1326,23 @@
       </c>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:25" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
+    <row r="8" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="24"/>
       <c r="B8" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="I8" s="4">
         <v>24</v>
@@ -1334,23 +1352,23 @@
       </c>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:25" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
+    <row r="9" spans="1:25" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="24"/>
       <c r="B9" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>108</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="I9" s="4">
         <v>24</v>
@@ -1360,23 +1378,23 @@
       </c>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
+    <row r="10" spans="1:25" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="24"/>
       <c r="B10" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>113</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>114</v>
       </c>
       <c r="I10" s="4">
         <v>12</v>
@@ -1389,16 +1407,16 @@
       </c>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="1:25" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
+    <row r="11" spans="1:25" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="24"/>
       <c r="B11" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="G11" s="22" t="str">
         <f t="shared" si="0"/>
@@ -1412,8 +1430,8 @@
       </c>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
+    <row r="12" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="24"/>
       <c r="B12" s="19" t="s">
         <v>21</v>
       </c>
@@ -1421,7 +1439,7 @@
         <v>22</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G12" s="22" t="str">
         <f t="shared" si="0"/>
@@ -1436,10 +1454,10 @@
       <c r="L12" s="5"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+    <row r="13" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="24"/>
       <c r="B13" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G13" s="22" t="str">
         <f t="shared" si="0"/>
@@ -1448,10 +1466,10 @@
       <c r="L13" s="5"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
+    <row r="14" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="24"/>
       <c r="B14" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G14" s="22" t="str">
         <f t="shared" si="0"/>
@@ -1459,23 +1477,23 @@
       </c>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
+    <row r="15" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="24"/>
       <c r="B15" s="19" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+      <c r="H15" s="10" t="s">
         <v>110</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>111</v>
       </c>
       <c r="I15" s="4">
         <v>24</v>
@@ -1486,8 +1504,8 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
+    <row r="16" spans="1:25" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="24"/>
       <c r="B16" s="19" t="s">
         <v>29</v>
       </c>
@@ -1502,7 +1520,7 @@
         <v>Datasheet</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I16" s="4">
         <v>24</v>
@@ -1514,24 +1532,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
+    <row r="17" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="24"/>
       <c r="B17" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G17" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I17" s="4">
         <v>24</v>
@@ -1540,13 +1558,13 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
+    <row r="18" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="24"/>
       <c r="B18" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>133</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -1555,69 +1573,69 @@
         <v>Datasheet</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>4</v>
       </c>
       <c r="K18" s="10"/>
     </row>
-    <row r="19" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
+    <row r="19" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="24"/>
       <c r="B19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="G19" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
+    <row r="20" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="24"/>
       <c r="B20" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="G20" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
+    <row r="21" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="24"/>
       <c r="G21" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
+    <row r="22" spans="1:13" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="24"/>
       <c r="B22" s="20"/>
       <c r="G22" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
-        <v>71</v>
+    <row r="23" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="24" t="s">
+        <v>70</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>14</v>
@@ -1626,7 +1644,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G23" s="22" t="str">
         <f t="shared" si="0"/>
@@ -1640,8 +1658,8 @@
       </c>
       <c r="L23" s="13"/>
     </row>
-    <row r="24" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="23"/>
+    <row r="24" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="24"/>
       <c r="B24" s="19" t="s">
         <v>26</v>
       </c>
@@ -1649,7 +1667,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G24" s="22" t="str">
         <f t="shared" si="0"/>
@@ -1663,16 +1681,16 @@
       </c>
       <c r="L24" s="13"/>
     </row>
-    <row r="25" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
+    <row r="25" spans="1:13" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="24"/>
       <c r="B25" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D25" s="4">
         <v>1</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G25" s="22" t="str">
         <f t="shared" si="0"/>
@@ -1686,39 +1704,41 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
+    <row r="26" spans="1:13" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="24"/>
       <c r="B26" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D26" s="4">
         <v>4</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G26" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
-      <c r="H26" s="9"/>
+      <c r="H26" s="9" t="s">
+        <v>166</v>
+      </c>
       <c r="I26" s="4">
         <v>12</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K26" s="10">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23"/>
+    <row r="27" spans="1:13" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="24"/>
       <c r="B27" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D27" s="4">
         <v>2</v>
@@ -1729,26 +1749,31 @@
         <v>Datasheet</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>4</v>
       </c>
       <c r="K27" s="10"/>
     </row>
-    <row r="28" spans="1:13" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
+    <row r="28" spans="1:13" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="24"/>
       <c r="B28" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>171</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G28" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
-      <c r="H28" s="14"/>
+      <c r="H28" s="23" t="s">
+        <v>170</v>
+      </c>
       <c r="I28" s="4">
         <v>24</v>
       </c>
@@ -1756,22 +1781,26 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
+    <row r="29" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="24"/>
       <c r="B29" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="C29" s="13"/>
+        <v>154</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>168</v>
+      </c>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="G29" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
-      <c r="H29" s="13"/>
+      <c r="H29" s="13" t="s">
+        <v>169</v>
+      </c>
       <c r="I29" s="13">
         <v>12</v>
       </c>
@@ -1782,8 +1811,8 @@
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
+    <row r="30" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="24"/>
       <c r="F30" s="9"/>
       <c r="G30" s="22" t="str">
         <f t="shared" si="0"/>
@@ -1792,13 +1821,13 @@
       <c r="H30" s="9"/>
       <c r="K30" s="10"/>
     </row>
-    <row r="31" spans="1:13" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
+    <row r="31" spans="1:13" ht="18.649999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="24"/>
       <c r="B31" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="G31" s="22" t="str">
         <f t="shared" si="0"/>
@@ -1811,15 +1840,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
-        <v>72</v>
+    <row r="32" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D32" s="4">
         <v>2</v>
@@ -1833,19 +1862,19 @@
         <v>Datasheet</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="24"/>
       <c r="B33" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D33" s="4">
         <v>4</v>
@@ -1859,19 +1888,19 @@
         <v>Datasheet</v>
       </c>
       <c r="H33" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="24"/>
+      <c r="B34" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="M33" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
@@ -1880,14 +1909,14 @@
         <v>1</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G34" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I34" s="4">
         <v>24</v>
@@ -1896,16 +1925,16 @@
         <v>0.6</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="24"/>
       <c r="B35" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D35" s="4">
         <v>2</v>
@@ -1919,19 +1948,19 @@
         <v>Datasheet</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="24"/>
       <c r="B36" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D36" s="4">
         <v>4</v>
@@ -1940,26 +1969,26 @@
         <v>3</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G36" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="24"/>
       <c r="B37" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D37" s="4">
         <v>1</v>
@@ -1969,19 +1998,19 @@
         <v>Datasheet</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="24"/>
       <c r="B38" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D38" s="4">
         <v>1</v>
@@ -1991,19 +2020,19 @@
         <v>Datasheet</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="24"/>
       <c r="B39" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D39" s="4">
         <v>4</v>
@@ -2016,19 +2045,19 @@
         <v>Datasheet</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="24"/>
       <c r="B40" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D40" s="4">
         <v>2</v>
@@ -2038,16 +2067,16 @@
         <v>Datasheet</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="24"/>
       <c r="B41" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D41" s="4">
         <v>1</v>
@@ -2057,10 +2086,10 @@
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="23"/>
+    <row r="42" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="24"/>
       <c r="B42" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D42" s="4">
         <v>1</v>
@@ -2070,25 +2099,25 @@
         <v>Datasheet</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="23"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="24"/>
       <c r="G43" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
-        <v>73</v>
+    <row r="44" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="24" t="s">
+        <v>72</v>
       </c>
       <c r="B44" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="D44" s="4">
         <v>3</v>
@@ -2098,13 +2127,13 @@
         <v>Datasheet</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="24"/>
       <c r="B45" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D45" s="4">
         <v>3</v>
@@ -2114,57 +2143,57 @@
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="23"/>
+    <row r="46" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="24"/>
       <c r="B46" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G46" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="23"/>
+    <row r="47" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="24"/>
       <c r="G47" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
+    <row r="48" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="24"/>
       <c r="G48" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
+    <row r="49" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="24"/>
       <c r="G49" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
+    <row r="50" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="24"/>
       <c r="G50" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="23"/>
+    <row r="51" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="24"/>
       <c r="G51" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="23" t="s">
-        <v>74</v>
+    <row r="52" spans="1:12" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="24" t="s">
+        <v>73</v>
       </c>
       <c r="B52" s="18" t="s">
         <v>2</v>
@@ -2186,8 +2215,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="23"/>
+    <row r="53" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="24"/>
       <c r="B53" s="19" t="s">
         <v>3</v>
       </c>
@@ -2202,8 +2231,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="23"/>
+    <row r="54" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="24"/>
       <c r="B54" s="19" t="s">
         <v>24</v>
       </c>
@@ -2212,110 +2241,110 @@
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="23"/>
+    <row r="55" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="24"/>
       <c r="G55" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="23" t="s">
+    <row r="56" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="B56" s="19" t="s">
+      <c r="G56" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>Datasheet</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="24"/>
+      <c r="B57" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G56" s="22" t="str">
-        <f t="shared" si="0"/>
-        <v>Datasheet</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
-      <c r="B57" s="19" t="s">
-        <v>148</v>
-      </c>
       <c r="G57" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="23" t="s">
-        <v>70</v>
+    <row r="58" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="24" t="s">
+        <v>69</v>
       </c>
       <c r="G58" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="23"/>
+    <row r="59" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="24"/>
       <c r="G59" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
+    <row r="60" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="24"/>
       <c r="G60" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="23"/>
+    <row r="61" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="24"/>
       <c r="G61" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="23"/>
+    <row r="62" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="24"/>
       <c r="G62" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="23"/>
+    <row r="63" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="24"/>
       <c r="G63" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
+    <row r="64" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="24"/>
       <c r="G64" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
+    <row r="65" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="24"/>
       <c r="G65" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
+    <row r="66" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="24"/>
       <c r="G66" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="23"/>
+    <row r="67" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="24"/>
       <c r="G67" s="22" t="str">
         <f t="shared" si="0"/>
         <v>Datasheet</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B68" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C68" s="13"/>
       <c r="D68" s="13"/>
@@ -2329,9 +2358,9 @@
         <v>1282.6599999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B69" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
@@ -2345,9 +2374,9 @@
         <v>668.8</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B70" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K70" s="13">
         <f>SUMIF(I3:I67,24,K3:K67)</f>
@@ -2369,8 +2398,11 @@
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="A56:A57"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H28" r:id="rId1" xr:uid="{25EE8CF7-0054-4A71-9349-0C96B7362F83}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2382,83 +2414,83 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.54296875" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2466,37 +2498,37 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -2514,117 +2546,117 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -2642,29 +2674,29 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.54296875" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" customWidth="1"/>
+    <col min="4" max="4" width="26.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2672,29 +2704,29 @@
         <v>36</v>
       </c>
       <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2702,12 +2734,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2715,77 +2747,77 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>24</v>
       </c>

</xml_diff>